<commit_message>
fixing test data and capture new object for case logout
</commit_message>
<xml_diff>
--- a/Data Files/Login/Login.xlsx
+++ b/Data Files/Login/Login.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12210"/>
+    <workbookView windowWidth="18350" windowHeight="6830"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -40,10 +40,10 @@
     <t>TD001</t>
   </si>
   <si>
-    <t>admintitan</t>
-  </si>
-  <si>
-    <t>Testing123@</t>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
   <si>
     <t>Positive</t>
@@ -52,10 +52,10 @@
     <t>Login Admin Succes</t>
   </si>
   <si>
-    <t>Success landing at Dashboard as Albertus Ganeshafiro</t>
-  </si>
-  <si>
-    <t>Albertus Ganeshafiro</t>
+    <t>Success landing at Dashboard Page</t>
+  </si>
+  <si>
+    <t>Dashboard Page</t>
   </si>
   <si>
     <t>TD002</t>
@@ -1250,14 +1250,14 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="12.1428571428571" customWidth="1"/>
-    <col min="3" max="4" width="13.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="17.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="12.1454545454545" customWidth="1"/>
+    <col min="3" max="4" width="13.1454545454545" customWidth="1"/>
+    <col min="5" max="5" width="17.7181818181818" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
   </cols>
@@ -1335,7 +1335,6 @@
       <c r="A4" t="s">
         <v>20</v>
       </c>
-      <c r="B4"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -1382,7 +1381,6 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6"/>
       <c r="D6" t="s">
         <v>16</v>
       </c>

</xml_diff>